<commit_message>
pas encore au point l'écriture sur un fichier existant
</commit_message>
<xml_diff>
--- a/COF_TEST.xlsx
+++ b/COF_TEST.xlsx
@@ -9,26 +9,64 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12135"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15795" windowHeight="6645"/>
   </bookViews>
   <sheets>
-    <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
+    <sheet name="unAutreNom" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="152511"/>
-  <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
-      <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-  </extLst>
 </workbook>
+</file>
+
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+  <si>
+    <t>id</t>
+  </si>
+  <si>
+    <t>NOM</t>
+  </si>
+  <si>
+    <t>JOUEUR</t>
+  </si>
+  <si>
+    <t>PROFIL</t>
+  </si>
+  <si>
+    <t>NIVEAU</t>
+  </si>
+  <si>
+    <t>RACE</t>
+  </si>
+  <si>
+    <t>SEXE</t>
+  </si>
+  <si>
+    <t>AGE</t>
+  </si>
+  <si>
+    <t>TAILLE</t>
+  </si>
+  <si>
+    <t>POIDS</t>
+  </si>
+</sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
-      <color theme="1"/>
+      <color indexed="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color indexed="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -54,8 +92,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -336,12 +380,152 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:M9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="4.7109375" style="1" customWidth="1"/>
+    <col min="2" max="11" width="10.42578125" style="1" customWidth="1"/>
+    <col min="12" max="16384" width="9.140625" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A1" s="1">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1">
+        <f>1+A1</f>
+        <v>1</v>
+      </c>
+      <c r="C1" s="1">
+        <f t="shared" ref="C1:M1" si="0">1+B1</f>
+        <v>2</v>
+      </c>
+      <c r="D1" s="1">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+      <c r="E1" s="1">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+      <c r="F1" s="1">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+      <c r="G1" s="1">
+        <f t="shared" si="0"/>
+        <v>6</v>
+      </c>
+      <c r="H1" s="1">
+        <f t="shared" si="0"/>
+        <v>7</v>
+      </c>
+      <c r="I1" s="1">
+        <f t="shared" si="0"/>
+        <v>8</v>
+      </c>
+      <c r="J1" s="1">
+        <f t="shared" si="0"/>
+        <v>9</v>
+      </c>
+      <c r="K1" s="1">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
+      <c r="L1" s="1">
+        <f t="shared" si="0"/>
+        <v>11</v>
+      </c>
+      <c r="M1" s="1">
+        <f t="shared" si="0"/>
+        <v>12</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A2" s="1">
+        <f>A1+1</f>
+        <v>1</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="H2" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="I2" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="J2" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="K2" s="2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A3" s="1">
+        <f t="shared" ref="A3:A9" si="1">A2+1</f>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A4" s="1">
+        <f t="shared" si="1"/>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A5" s="1">
+        <f t="shared" si="1"/>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A6" s="1">
+        <f t="shared" si="1"/>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A7" s="1">
+        <f t="shared" si="1"/>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A8" s="1">
+        <f t="shared" si="1"/>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A9" s="1">
+        <f t="shared" si="1"/>
+        <v>8</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>